<commit_message>
updated the coverpage and transmittal templates
</commit_message>
<xml_diff>
--- a/templates/Transmittal.xlsx
+++ b/templates/Transmittal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n01632161\PyCharmMiscProject\psproject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n01632161\PyCharmMiscProject\gitproject\PSDemo\psc-submittals-git\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E4AC47F-86D0-4CDD-9CC7-1F98778E37E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AFB4A5-66FB-402F-AFCE-BFCC329F5708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{B1C04B84-DF5F-4C36-9887-95807CCD083B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>TO:</t>
   </si>
@@ -162,6 +162,18 @@
   </si>
   <si>
     <t>Field Report</t>
+  </si>
+  <si>
+    <t>{{DATE}}</t>
+  </si>
+  <si>
+    <t>{{ENGINEER_NAME}}</t>
+  </si>
+  <si>
+    <t>{{ENGINEER_ADDRESS}}</t>
+  </si>
+  <si>
+    <t>{{PSCC_JOB_NO}}</t>
   </si>
 </sst>
 </file>
@@ -823,7 +835,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" defaultGridColor="0" colorId="22" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81640625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -871,14 +883,20 @@
       <c r="F5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="26"/>
+      <c r="G5" s="26" t="s">
+        <v>42</v>
+      </c>
       <c r="H5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="25"/>
+      <c r="I5" s="25" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="8"/>
+      <c r="A6" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -890,7 +908,9 @@
       <c r="I6" s="11"/>
     </row>
     <row r="7" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A7" s="8"/>
+      <c r="A7" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>

</xml_diff>